<commit_message>
added BOM for 1.7
</commit_message>
<xml_diff>
--- a/cosmicpi_1.6_enhanced.xlsx
+++ b/cosmicpi_1.6_enhanced.xlsx
@@ -5,7 +5,7 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdevine\Downloads\cosmicmarch\cosmicpi_1.6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdevine\Downloads\CosmicPiV1.7PCB-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2462,8 +2462,8 @@
   </sheetPr>
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>